<commit_message>
currently finishing vacation for hr
</commit_message>
<xml_diff>
--- a/public/BulkFormat.xlsx
+++ b/public/BulkFormat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawk\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E9DFBD2-EDFB-4051-8BC7-7B5ECF5A105C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988B2490-4CA4-4297-A852-38967C664499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7185" yWindow="3105" windowWidth="21600" windowHeight="11295" xr2:uid="{393F6449-7D06-4F82-844C-9C3598695434}"/>
+    <workbookView xWindow="-27255" yWindow="2640" windowWidth="21600" windowHeight="11835" xr2:uid="{393F6449-7D06-4F82-844C-9C3598695434}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>email</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>birthDate</t>
   </si>
 </sst>
 </file>
@@ -104,8 +107,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8820F3B4-0EF6-4B1D-A5D1-4B9498A7CF17}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,12 +440,13 @@
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,12 +472,15 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>